<commit_message>
B time:10 comment: weighted past individual projects with last semester's project to create new all inclusive PROBE table
</commit_message>
<xml_diff>
--- a/deliverables/t3/probe/t2Probe.xlsx
+++ b/deliverables/t3/probe/t2Probe.xlsx
@@ -168,16 +168,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.96</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.266666666666666</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,11 +255,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131847296"/>
-        <c:axId val="131848832"/>
+        <c:axId val="53116928"/>
+        <c:axId val="53118464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131847296"/>
+        <c:axId val="53116928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131848832"/>
+        <c:crossAx val="53118464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -276,7 +276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131848832"/>
+        <c:axId val="53118464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,7 +287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131847296"/>
+        <c:crossAx val="53116928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -631,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,26 +679,26 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
+      <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="J8" s="3"/>
@@ -719,10 +719,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="1">
+      <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -732,27 +732,23 @@
         <v>2</v>
       </c>
       <c r="L9" s="4">
-        <f>AVERAGE(C6:C20)</f>
-        <v>4.5999999999999996</v>
+        <v>4</v>
       </c>
       <c r="M9" s="4">
-        <f>AVERAGE(E22:E46)</f>
-        <v>10.96</v>
+        <v>7</v>
       </c>
       <c r="N9" s="4">
-        <f>AVERAGE(G47:G61)</f>
-        <v>24.266666666666666</v>
+        <v>18</v>
       </c>
       <c r="O9" s="4">
-        <f>AVERAGE(I62:I66)</f>
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="1">
+      <c r="B10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -763,448 +759,454 @@
         <v>4.5</v>
       </c>
       <c r="L10" s="4">
-        <f>AVERAGE(D6:D20)</f>
+        <f>AVERAGE(B6:B20)</f>
         <v>4.5333333333333332</v>
       </c>
       <c r="M10" s="4">
-        <f>AVERAGE(F22:F46)</f>
+        <f>AVERAGE(B21:B45)</f>
         <v>3.7826086956521738</v>
       </c>
       <c r="N10" s="4">
-        <f>AVERAGE(H47:H61)</f>
+        <f>AVERAGE(B46:B60)</f>
         <v>2.4615384615384617</v>
       </c>
       <c r="O10" s="4">
-        <f>AVERAGE(J62:J66)</f>
+        <f>AVERAGE(B61:B65)</f>
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
+      <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="1">
+      <c r="B11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="2">
+      <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="2">
+      <c r="B12" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="2">
+      <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="B13" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
+      <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="B14" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
+      <c r="A15" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="B15" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+      <c r="A16" s="1">
         <v>6</v>
       </c>
-      <c r="D16" s="1">
+      <c r="B16" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>6</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="2">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>6</v>
       </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="2">
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="B19" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>6</v>
       </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>6</v>
       </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="2">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>7</v>
       </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="2">
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>7</v>
       </c>
-      <c r="F24" s="2">
+      <c r="B23" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="1">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>7</v>
       </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="1">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>8</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="1">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>8</v>
       </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="1">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>8</v>
       </c>
-      <c r="F28" s="1">
+      <c r="B27" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="1">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>8</v>
       </c>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="1">
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>10</v>
       </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="1">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>10</v>
       </c>
-      <c r="F31" s="1">
+      <c r="B30" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>10</v>
       </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="2">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>10</v>
       </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="1">
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>10</v>
       </c>
-      <c r="F34" s="1">
+      <c r="B33" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="1">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>11</v>
       </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E36" s="1">
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>11</v>
       </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="1">
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>12</v>
       </c>
-      <c r="F37" s="1">
+      <c r="B36" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="1">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>13</v>
       </c>
-      <c r="F38" s="1">
+      <c r="B37" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="1">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>13</v>
       </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="1">
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>14</v>
       </c>
-      <c r="F40" s="1">
+      <c r="B39" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>14</v>
       </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E42" s="1">
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>15</v>
       </c>
-      <c r="F42" s="1">
+      <c r="B41" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E43" s="1">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>15</v>
       </c>
-      <c r="F43" s="1">
+      <c r="B42" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="1">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>15</v>
       </c>
-      <c r="F44" s="1">
+      <c r="B43" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E45" s="1">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>16</v>
       </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E46" s="1">
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>16</v>
       </c>
-      <c r="F46" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="1">
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>16</v>
       </c>
-      <c r="H47" s="1">
+      <c r="B46" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="G48" s="1">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>17</v>
       </c>
-      <c r="H48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G49" s="1">
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>18</v>
       </c>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G50" s="1">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>19</v>
       </c>
-      <c r="H50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G51" s="1">
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>20</v>
       </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G52" s="2">
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>21</v>
       </c>
-      <c r="H52" s="2">
+      <c r="B51" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G53" s="1">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>21</v>
       </c>
-      <c r="H53" s="1">
+      <c r="B52" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G54" s="1">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>21</v>
       </c>
-      <c r="H54" s="1">
+      <c r="B53" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G55" s="1">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>23</v>
       </c>
-      <c r="H55" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G56" s="1">
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>24</v>
       </c>
-      <c r="H56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G57" s="1">
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>26</v>
       </c>
-      <c r="H57" s="1">
+      <c r="B56" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G58" s="2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>27</v>
       </c>
-      <c r="H58" s="2">
+      <c r="B57" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G59" s="1">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>33</v>
       </c>
-      <c r="H59" s="1">
+      <c r="B58" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G60" s="1">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>38</v>
       </c>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G61" s="1">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>40</v>
       </c>
-      <c r="H61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="I62" s="1">
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>41</v>
       </c>
-      <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="I63" s="1">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>43</v>
       </c>
-      <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="I64" s="2">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>45</v>
       </c>
-      <c r="J64" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I65" s="1">
+      <c r="B63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>58</v>
       </c>
-      <c r="J65" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I66" s="1">
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>58</v>
       </c>
-      <c r="J66" s="1">
+      <c r="B65" s="1">
         <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f>SUM(A6:A66)</f>
+        <v>952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROBE table file looked corrupt
</commit_message>
<xml_diff>
--- a/deliverables/t3/probe/t2Probe.xlsx
+++ b/deliverables/t3/probe/t2Probe.xlsx
@@ -255,11 +255,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53116928"/>
-        <c:axId val="53118464"/>
+        <c:axId val="67006464"/>
+        <c:axId val="67008000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53116928"/>
+        <c:axId val="67006464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53118464"/>
+        <c:crossAx val="67008000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -276,7 +276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53118464"/>
+        <c:axId val="67008000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,7 +287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53116928"/>
+        <c:crossAx val="67006464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -634,7 +634,7 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,6 +1215,9 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="L10:O10" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>